<commit_message>
added trello to README
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D356FDF2-F1AE-42CD-AB14-292726F1FE4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481E6CC5-8D59-4172-AEC0-154CB80D0C40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -805,6 +805,32 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
+      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
@@ -976,32 +1002,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1324,12 +1324,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Beskrivelse af milepæle" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Kategori" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tildelt til" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Beskrivelse af milepæle" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Kategori" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tildelt til" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Gang"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" totalsRowDxfId="10" dataCellStyle="Dato"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Antal dage" totalsRowFunction="sum" totalsRowDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" totalsRowDxfId="1" dataCellStyle="Dato"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Antal dage" totalsRowFunction="sum" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gantt-tabeltypografi" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1608,7 +1608,7 @@
   </sheetPr>
   <dimension ref="A1:BL35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -8194,39 +8194,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BL33">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AM4">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>I$5&lt;=EOMONTH($I$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BL4">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>AND(J$5&lt;=EOMONTH($I$5,2),J$5&gt;EOMONTH($I$5,0),J$5&gt;EOMONTH($I$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BL4">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(I$5&lt;=EOMONTH($I$5,1),I$5&gt;EOMONTH($I$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BL32">
-    <cfRule type="expression" dxfId="4" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
       <formula>AND($C8="Lav risiko",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="43" stopIfTrue="1">
       <formula>AND($C8="Høj risiko",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="61" stopIfTrue="1">
       <formula>AND($C8="På rette spor",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="62" stopIfTrue="1">
       <formula>AND($C8="Mellem risiko",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="63" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>